<commit_message>
Changed ArrayList to List
</commit_message>
<xml_diff>
--- a/Programming Challenge.xlsx
+++ b/Programming Challenge.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8295" uniqueCount="970">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8393" uniqueCount="972">
   <si>
     <t>Emma</t>
   </si>
@@ -2928,6 +2928,12 @@
   </si>
   <si>
     <t>{"Rumor ID":4,"Rumor Travel Time":2725,"Calculation Time":2}</t>
+  </si>
+  <si>
+    <t>{"Rumor ID":11,"Rumor Travel Time":5748,"Calculation Time":1}</t>
+  </si>
+  <si>
+    <t>{"Rumor ID":44,"Rumor Travel Time":6268,"Calculation Time":26}</t>
   </si>
 </sst>
 </file>
@@ -32888,7 +32894,7 @@
         <v>673</v>
       </c>
       <c r="F4" t="s">
-        <v>968</v>
+        <v>674</v>
       </c>
       <c r="H4" t="s">
         <v>670</v>
@@ -32909,7 +32915,7 @@
         <v>675</v>
       </c>
       <c r="F5" t="s">
-        <v>904</v>
+        <v>771</v>
       </c>
       <c r="H5" t="s">
         <v>671</v>
@@ -32930,7 +32936,7 @@
         <v>677</v>
       </c>
       <c r="F6" t="s">
-        <v>802</v>
+        <v>678</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -32948,7 +32954,7 @@
         <v>679</v>
       </c>
       <c r="F7" t="s">
-        <v>969</v>
+        <v>680</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -32966,7 +32972,7 @@
         <v>681</v>
       </c>
       <c r="F8" t="s">
-        <v>788</v>
+        <v>682</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -32984,7 +32990,7 @@
         <v>683</v>
       </c>
       <c r="F9" t="s">
-        <v>817</v>
+        <v>789</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -33020,7 +33026,7 @@
         <v>687</v>
       </c>
       <c r="F11" t="s">
-        <v>688</v>
+        <v>907</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -33038,7 +33044,7 @@
         <v>689</v>
       </c>
       <c r="F12" t="s">
-        <v>690</v>
+        <v>955</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -33056,7 +33062,7 @@
         <v>691</v>
       </c>
       <c r="F13" t="s">
-        <v>811</v>
+        <v>773</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -33074,7 +33080,7 @@
         <v>693</v>
       </c>
       <c r="F14" t="s">
-        <v>694</v>
+        <v>970</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -33092,7 +33098,7 @@
         <v>695</v>
       </c>
       <c r="F15" t="s">
-        <v>797</v>
+        <v>775</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -33128,7 +33134,7 @@
         <v>699</v>
       </c>
       <c r="F17" t="s">
-        <v>776</v>
+        <v>700</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -33164,7 +33170,7 @@
         <v>703</v>
       </c>
       <c r="F19" t="s">
-        <v>704</v>
+        <v>799</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -33182,7 +33188,7 @@
         <v>705</v>
       </c>
       <c r="F20" t="s">
-        <v>706</v>
+        <v>869</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -33200,7 +33206,7 @@
         <v>707</v>
       </c>
       <c r="F21" t="s">
-        <v>708</v>
+        <v>800</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -33218,7 +33224,7 @@
         <v>709</v>
       </c>
       <c r="F22" t="s">
-        <v>710</v>
+        <v>834</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -33362,7 +33368,7 @@
         <v>725</v>
       </c>
       <c r="F30" t="s">
-        <v>780</v>
+        <v>726</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
@@ -33380,7 +33386,7 @@
         <v>727</v>
       </c>
       <c r="F31" t="s">
-        <v>781</v>
+        <v>728</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -33578,7 +33584,7 @@
         <v>749</v>
       </c>
       <c r="F42" t="s">
-        <v>750</v>
+        <v>801</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
@@ -33614,7 +33620,7 @@
         <v>753</v>
       </c>
       <c r="F44" t="s">
-        <v>784</v>
+        <v>754</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
@@ -33668,7 +33674,7 @@
         <v>759</v>
       </c>
       <c r="F47" t="s">
-        <v>785</v>
+        <v>971</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>